<commit_message>
Docs: Atualização das atividade do Backlog final
</commit_message>
<xml_diff>
--- a/Backlog HerpSafe/Product backlog.xlsx
+++ b/Backlog HerpSafe/Product backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ezequiel\Downloads\HerpSafe-Sprint-2\Backlog HerpSafe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\HerpSafe-Sprint-2\Backlog HerpSafe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813BBE0B-4DB8-4001-A0C0-6ADCAB413461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5980D96F-75CF-4032-9B62-4580D829A25F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10140" yWindow="0" windowWidth="10440" windowHeight="10905" xr2:uid="{AB679324-3DC8-4F8A-B107-B10CD92536BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AB679324-3DC8-4F8A-B107-B10CD92536BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="163">
   <si>
     <t>Tipo</t>
   </si>
@@ -177,9 +177,6 @@
     <t>Concluído</t>
   </si>
   <si>
-    <t>Pendente</t>
-  </si>
-  <si>
     <t>Opção logo abaixo do formulário de login para recuperar a senha. Ao acessar, solicitar o e-mail registrado. Caso seja encontrado nos registros, um e-mail será enviado ao e-mail cadastrado com instruções para recuperação.</t>
   </si>
   <si>
@@ -286,9 +283,6 @@
   </si>
   <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>Backlog</t>
   </si>
   <si>
     <t>Entregável ou Requisito</t>
@@ -1095,9 +1089,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{831A3FE2-A405-481B-8C5B-5096A2CC35E1}">
   <dimension ref="B1:L59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="35.1" customHeight="1" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -1146,7 +1140,7 @@
         <v>1</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>41</v>
@@ -1154,7 +1148,7 @@
     </row>
     <row r="2" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>26</v>
@@ -1170,7 +1164,7 @@
         <v>5</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>7</v>
@@ -1190,7 +1184,7 @@
     </row>
     <row r="3" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>29</v>
@@ -1206,7 +1200,7 @@
         <v>8</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>7</v>
@@ -1226,7 +1220,7 @@
     </row>
     <row r="4" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>30</v>
@@ -1242,7 +1236,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>7</v>
@@ -1262,7 +1256,7 @@
     </row>
     <row r="5" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>31</v>
@@ -1278,7 +1272,7 @@
         <v>5</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>7</v>
@@ -1298,7 +1292,7 @@
     </row>
     <row r="6" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>27</v>
@@ -1314,7 +1308,7 @@
         <v>13</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>7</v>
@@ -1334,7 +1328,7 @@
     </row>
     <row r="7" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>33</v>
@@ -1350,7 +1344,7 @@
         <v>8</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>7</v>
@@ -1370,7 +1364,7 @@
     </row>
     <row r="8" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>34</v>
@@ -1386,7 +1380,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>7</v>
@@ -1406,7 +1400,7 @@
     </row>
     <row r="9" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>35</v>
@@ -1422,7 +1416,7 @@
         <v>5</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>7</v>
@@ -1442,7 +1436,7 @@
     </row>
     <row r="10" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>28</v>
@@ -1458,7 +1452,7 @@
         <v>13</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>7</v>
@@ -1478,7 +1472,7 @@
     </row>
     <row r="11" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>36</v>
@@ -1494,7 +1488,7 @@
         <v>8</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>7</v>
@@ -1514,7 +1508,7 @@
     </row>
     <row r="12" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>37</v>
@@ -1530,7 +1524,7 @@
         <v>8</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>7</v>
@@ -1550,7 +1544,7 @@
     </row>
     <row r="13" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>38</v>
@@ -1566,7 +1560,7 @@
         <v>8</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>7</v>
@@ -1586,7 +1580,7 @@
     </row>
     <row r="14" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>39</v>
@@ -1602,7 +1596,7 @@
         <v>3</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>7</v>
@@ -1622,7 +1616,7 @@
     </row>
     <row r="15" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>42</v>
@@ -1638,7 +1632,7 @@
         <v>5</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>7</v>
@@ -1658,7 +1652,7 @@
     </row>
     <row r="16" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>40</v>
@@ -1674,7 +1668,7 @@
         <v>3</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>7</v>
@@ -1694,7 +1688,7 @@
     </row>
     <row r="17" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>40</v>
@@ -1710,7 +1704,7 @@
         <v>3</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>7</v>
@@ -1730,10 +1724,10 @@
     </row>
     <row r="18" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>23</v>
@@ -1746,7 +1740,7 @@
         <v>3</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>7</v>
@@ -1758,7 +1752,7 @@
         <v>10</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="L18" s="4" t="s">
         <v>43</v>
@@ -1766,10 +1760,10 @@
     </row>
     <row r="19" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>23</v>
@@ -1782,7 +1776,7 @@
         <v>5</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H19" s="4" t="s">
         <v>7</v>
@@ -1794,7 +1788,7 @@
         <v>10</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="L19" s="4" t="s">
         <v>43</v>
@@ -1802,10 +1796,10 @@
     </row>
     <row r="20" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>23</v>
@@ -1818,7 +1812,7 @@
         <v>13</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>7</v>
@@ -1830,7 +1824,7 @@
         <v>10</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="L20" s="4" t="s">
         <v>43</v>
@@ -1838,10 +1832,10 @@
     </row>
     <row r="21" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>23</v>
@@ -1854,7 +1848,7 @@
         <v>5</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>7</v>
@@ -1866,7 +1860,7 @@
         <v>10</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="L21" s="4" t="s">
         <v>43</v>
@@ -1874,10 +1868,10 @@
     </row>
     <row r="22" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>23</v>
@@ -1890,7 +1884,7 @@
         <v>3</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>7</v>
@@ -1902,7 +1896,7 @@
         <v>10</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L22" s="4" t="s">
         <v>43</v>
@@ -1910,10 +1904,10 @@
     </row>
     <row r="23" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>23</v>
@@ -1926,7 +1920,7 @@
         <v>5</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>7</v>
@@ -1938,7 +1932,7 @@
         <v>10</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L23" s="4" t="s">
         <v>43</v>
@@ -1946,10 +1940,10 @@
     </row>
     <row r="24" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>23</v>
@@ -1962,7 +1956,7 @@
         <v>8</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H24" s="4" t="s">
         <v>7</v>
@@ -1974,7 +1968,7 @@
         <v>10</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L24" s="4" t="s">
         <v>43</v>
@@ -1982,10 +1976,10 @@
     </row>
     <row r="25" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>23</v>
@@ -1998,7 +1992,7 @@
         <v>8</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H25" s="4" t="s">
         <v>7</v>
@@ -2010,7 +2004,7 @@
         <v>10</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L25" s="4" t="s">
         <v>43</v>
@@ -2018,10 +2012,10 @@
     </row>
     <row r="26" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>23</v>
@@ -2034,7 +2028,7 @@
         <v>8</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H26" s="4" t="s">
         <v>7</v>
@@ -2046,7 +2040,7 @@
         <v>10</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L26" s="4" t="s">
         <v>43</v>
@@ -2054,10 +2048,10 @@
     </row>
     <row r="27" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>23</v>
@@ -2070,7 +2064,7 @@
         <v>5</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>7</v>
@@ -2082,7 +2076,7 @@
         <v>10</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L27" s="4" t="s">
         <v>43</v>
@@ -2090,10 +2084,10 @@
     </row>
     <row r="28" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>23</v>
@@ -2106,7 +2100,7 @@
         <v>5</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H28" s="4" t="s">
         <v>7</v>
@@ -2118,7 +2112,7 @@
         <v>10</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L28" s="4" t="s">
         <v>43</v>
@@ -2126,7 +2120,7 @@
     </row>
     <row r="29" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>32</v>
@@ -2142,7 +2136,7 @@
         <v>8</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H29" s="4" t="s">
         <v>7</v>
@@ -2154,18 +2148,18 @@
         <v>8</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>23</v>
@@ -2178,7 +2172,7 @@
         <v>5</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H30" s="4" t="s">
         <v>7</v>
@@ -2190,18 +2184,18 @@
         <v>10</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>23</v>
@@ -2214,7 +2208,7 @@
         <v>13</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H31" s="4" t="s">
         <v>7</v>
@@ -2226,18 +2220,18 @@
         <v>10</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>23</v>
@@ -2250,7 +2244,7 @@
         <v>8</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H32" s="4" t="s">
         <v>7</v>
@@ -2262,18 +2256,18 @@
         <v>10</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>23</v>
@@ -2286,7 +2280,7 @@
         <v>5</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H33" s="4" t="s">
         <v>7</v>
@@ -2298,7 +2292,7 @@
         <v>10</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L33" s="4" t="s">
         <v>43</v>
@@ -2306,10 +2300,10 @@
     </row>
     <row r="34" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>23</v>
@@ -2322,7 +2316,7 @@
         <v>8</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H34" s="4" t="s">
         <v>7</v>
@@ -2334,7 +2328,7 @@
         <v>10</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L34" s="4" t="s">
         <v>43</v>
@@ -2342,10 +2336,10 @@
     </row>
     <row r="35" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>23</v>
@@ -2358,7 +2352,7 @@
         <v>8</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H35" s="4" t="s">
         <v>7</v>
@@ -2370,18 +2364,18 @@
         <v>10</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>23</v>
@@ -2394,7 +2388,7 @@
         <v>8</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H36" s="4" t="s">
         <v>7</v>
@@ -2406,18 +2400,18 @@
         <v>10</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>23</v>
@@ -2430,7 +2424,7 @@
         <v>8</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H37" s="4" t="s">
         <v>7</v>
@@ -2442,21 +2436,21 @@
         <v>10</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>14</v>
@@ -2466,7 +2460,7 @@
         <v>3</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H38" s="4" t="s">
         <v>7</v>
@@ -2478,21 +2472,21 @@
         <v>10</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>14</v>
@@ -2502,7 +2496,7 @@
         <v>3</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H39" s="4" t="s">
         <v>7</v>
@@ -2514,18 +2508,18 @@
         <v>10</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>23</v>
@@ -2538,7 +2532,7 @@
         <v>8</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H40" s="4" t="s">
         <v>7</v>
@@ -2550,21 +2544,21 @@
         <v>10</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="L40" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>17</v>
@@ -2574,33 +2568,33 @@
         <v>13</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H41" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L41" s="4" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
     </row>
     <row r="42" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>17</v>
@@ -2610,33 +2604,33 @@
         <v>13</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H42" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>16</v>
@@ -2646,33 +2640,33 @@
         <v>8</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H43" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L43" s="4" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>17</v>
@@ -2682,30 +2676,30 @@
         <v>13</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H44" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L44" s="4" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>23</v>
@@ -2718,33 +2712,33 @@
         <v>8</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H45" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L45" s="4" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C46" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D46" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>16</v>
@@ -2754,33 +2748,33 @@
         <v>8</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H46" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L46" s="4" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>17</v>
@@ -2790,33 +2784,33 @@
         <v>13</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H47" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L47" s="4" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>15</v>
@@ -2826,33 +2820,33 @@
         <v>5</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H48" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L48" s="4" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>17</v>
@@ -2862,33 +2856,33 @@
         <v>13</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H49" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L49" s="4" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>16</v>
@@ -2898,33 +2892,33 @@
         <v>8</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H50" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L50" s="4" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
     </row>
     <row r="51" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>15</v>
@@ -2934,33 +2928,33 @@
         <v>5</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H51" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
     </row>
     <row r="52" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>16</v>
@@ -2970,33 +2964,33 @@
         <v>8</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H52" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K52" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L52" s="4" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
     </row>
     <row r="53" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>16</v>
@@ -3006,33 +3000,33 @@
         <v>8</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H53" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K53" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>17</v>
@@ -3042,33 +3036,33 @@
         <v>13</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H54" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K54" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L54" s="4" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
     </row>
     <row r="55" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>16</v>
@@ -3078,22 +3072,22 @@
         <v>8</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H55" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K55" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L55" s="4" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3153,7 +3147,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="6:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3167,7 +3161,7 @@
     </row>
     <row r="10" spans="6:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F10" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G10" s="5">
         <f>SUMIF('Product Backlog'!K:K,'Fibonacci por Sprint'!F10,'Product Backlog'!F:F)</f>
@@ -3176,7 +3170,7 @@
     </row>
     <row r="11" spans="6:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F11" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G11" s="5">
         <f>SUMIF('Product Backlog'!K:K,'Fibonacci por Sprint'!F11,'Product Backlog'!F:F)</f>
@@ -3185,7 +3179,7 @@
     </row>
     <row r="12" spans="6:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F12" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G12" s="5">
         <f>SUMIF('Product Backlog'!K:K,'Fibonacci por Sprint'!F12,'Product Backlog'!F:F)</f>
@@ -3194,7 +3188,7 @@
     </row>
     <row r="13" spans="6:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F13" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G13" s="5">
         <f>SUMIF('Product Backlog'!K:K,'Fibonacci por Sprint'!F13,'Product Backlog'!F:F)</f>
@@ -3203,7 +3197,7 @@
     </row>
     <row r="14" spans="6:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F14" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G14" s="5">
         <f>SUMIF('Product Backlog'!K:K,'Fibonacci por Sprint'!F14,'Product Backlog'!F:F)</f>
@@ -3235,7 +3229,7 @@
         <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3243,7 +3237,7 @@
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3251,7 +3245,7 @@
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3259,7 +3253,7 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3267,7 +3261,7 @@
         <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3275,7 +3269,7 @@
         <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3283,7 +3277,7 @@
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3291,7 +3285,7 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3299,7 +3293,7 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3307,7 +3301,7 @@
         <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -3397,16 +3391,16 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>